<commit_message>
Data Exporter 3rd version (corrupted file)
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -20,10 +20,10 @@
     <t>Data de emissão:</t>
   </si>
   <si>
-    <t>29/08/2022</t>
-  </si>
-  <si>
-    <t>17:07:13</t>
+    <t>30/08/2022</t>
+  </si>
+  <si>
+    <t>08:44:47</t>
   </si>
   <si>
     <t>Data de publicação:</t>

</xml_diff>